<commit_message>
Updated afitabl: added HistoryID, Version columns.
</commit_message>
<xml_diff>
--- a/source/Switch/afitabl.xlsx
+++ b/source/Switch/afitabl.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\design\open\switch\source\Switch\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA7C861-F1AC-4684-BD57-897AD0C43CFE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="390" windowWidth="28275" windowHeight="12315"/>
+    <workbookView xWindow="360" yWindow="390" windowWidth="28275" windowHeight="12315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="afitabl" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>LastWriteTime</t>
   </si>
@@ -59,12 +65,30 @@
   </si>
   <si>
     <t>HistoryID</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>3.4.1.113</t>
+  </si>
+  <si>
+    <t>3.3.1.110</t>
+  </si>
+  <si>
+    <t>3.5.2.114</t>
+  </si>
+  <si>
+    <t>3.6.0.0</t>
+  </si>
+  <si>
+    <t>alfa1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -548,48 +572,48 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -597,12 +621,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -644,7 +671,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -677,9 +704,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -712,6 +756,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -887,19 +948,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="109.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -915,8 +978,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -932,8 +998,11 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -949,8 +1018,11 @@
       <c r="E3" t="s">
         <v>5</v>
       </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -966,8 +1038,11 @@
       <c r="E4" t="s">
         <v>6</v>
       </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -983,8 +1058,11 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1000,8 +1078,11 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1017,8 +1098,11 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1034,8 +1118,11 @@
       <c r="E8" t="s">
         <v>10</v>
       </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1051,8 +1138,11 @@
       <c r="E9" t="s">
         <v>11</v>
       </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1068,8 +1158,11 @@
       <c r="E10" t="s">
         <v>12</v>
       </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1084,6 +1177,9 @@
       </c>
       <c r="E11" t="s">
         <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>